<commit_message>
Refitting NCDEs to individual patients (for manuscript figure)
</commit_message>
<xml_diff>
--- a/Results/Classification/Augmented Data/Full VPOP Classification/By Diagnosis/Control 0 (30, 11, 3, 38, 29)/MDD 0 (41, 8, 15, 16, 33)/NCDE_32nodes_Uniform0.05Virtual_Control(30, 11, 3, 38, 29)_MDD(41, 8, 15, 16, 33)_100perPatient_batchsize200_200maxITER_StandardizeAll_smoothing0_dropout0.0.xlsx
+++ b/Results/Classification/Augmented Data/Full VPOP Classification/By Diagnosis/Control 0 (30, 11, 3, 38, 29)/MDD 0 (41, 8, 15, 16, 33)/NCDE_32nodes_Uniform0.05Virtual_Control(30, 11, 3, 38, 29)_MDD(41, 8, 15, 16, 33)_100perPatient_batchsize200_200maxITER_StandardizeAll_smoothing0_dropout0.0.xlsx
@@ -453,13 +453,13 @@
         <v>100</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2.589448061374433E-189</v>
+        <v>0.9436880108715421</v>
       </c>
       <c r="E2">
-        <v>2.589448061374433E-189</v>
+        <v>0.9436880108715421</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -467,13 +467,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3.409454019658735E-188</v>
+        <v>0.5231981645955388</v>
       </c>
       <c r="E3">
-        <v>3.409454019658735E-188</v>
+        <v>0.5231981645955388</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -484,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>2.340115682762554E-197</v>
+        <v>7.588704048205964E-22</v>
       </c>
       <c r="E4">
-        <v>2.340115682762554E-197</v>
+        <v>7.588704048205964E-22</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -495,13 +495,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.01007968507949718</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.01007968507949718</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -512,10 +512,10 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>2.300151029592332E-133</v>
+        <v>0.009665622499053917</v>
       </c>
       <c r="E6">
-        <v>2.300151029592332E-133</v>
+        <v>0.009665622499053917</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -526,10 +526,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>5.141228057332627E-185</v>
+        <v>0.2934955359589477</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.7065044640410523</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -540,10 +540,10 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1.120859776408915E-179</v>
+        <v>1.091631452558186E-16</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -554,10 +554,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>6.196118980658183E-192</v>
+        <v>0.2460049466252581</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.7539950533747419</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -565,13 +565,13 @@
         <v>14</v>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>9.072030346907286E-181</v>
+        <v>0.9145149689747876</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.08548503102521243</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -582,13 +582,13 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>2.773730179944484E-141</v>
+        <v>0.03527451822687483</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0.9647254817731252</v>
       </c>
       <c r="F11">
-        <v>235.6986541748047</v>
+        <v>4.645328998565674</v>
       </c>
       <c r="G11">
         <v>0.4</v>
@@ -602,13 +602,13 @@
         <v>200</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>4.362312954353557E-230</v>
+        <v>0.9944810817313268</v>
       </c>
       <c r="E12">
-        <v>4.362312954353557E-230</v>
+        <v>0.9944810817313268</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -619,10 +619,10 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1.488180512215247E-230</v>
+        <v>0.3627090294370143</v>
       </c>
       <c r="E13">
-        <v>1.488180512215247E-230</v>
+        <v>0.3627090294370143</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -633,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>5.769634028113341E-243</v>
+        <v>6.820333666331986E-18</v>
       </c>
       <c r="E14">
-        <v>5.769634028113341E-243</v>
+        <v>6.820333666331986E-18</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -644,13 +644,13 @@
         <v>9</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.0001351607060775824</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0.0001351607060775824</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -658,13 +658,13 @@
         <v>10</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0.000378708834058626</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.000378708834058626</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -675,10 +675,10 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1.889565542396509E-228</v>
+        <v>0.227710223963856</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.772289776036144</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -689,10 +689,10 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>6.412389505168851E-213</v>
+        <v>9.716580453033788E-10</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.9999999990283419</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -703,10 +703,10 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>2.008307087085328E-234</v>
+        <v>0.05760872615149847</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0.9423912738485015</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -714,13 +714,13 @@
         <v>14</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>5.87290177500898E-225</v>
+        <v>0.9999999998825968</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>1.174031982742463E-10</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -728,19 +728,19 @@
         <v>15</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.02100077495614618</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.9789992250438538</v>
       </c>
       <c r="F21">
-        <v>302.9453430175781</v>
+        <v>3.459959506988525</v>
       </c>
       <c r="G21">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>